<commit_message>
cập nhật ttcn và đặt bàn
</commit_message>
<xml_diff>
--- a/TaiLieu/duanxuat/BaoCaoTonKhoNguyenLieu_20251102_0052.xlsx
+++ b/TaiLieu/duanxuat/BaoCaoTonKhoNguyenLieu_20251102_0052.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>BÁO CÁO TỔNG QUAN KHO</t>
   </si>
   <si>
-    <t>Báo cáo tạo lúc: 02/11/2025 00:52</t>
+    <t>Báo cáo tạo lúc: 07/11/2025 09:47</t>
   </si>
   <si>
     <t>CHỈ SỐ QUAN TRỌNG</t>
@@ -53,7 +53,7 @@
     <t>TinhTrang</t>
   </si>
   <si>
-    <t>Bột Cacao</t>
+    <t>Bột Matcha Nhật Bản</t>
   </si>
   <si>
     <t>kg</t>
@@ -62,19 +62,37 @@
     <t>Đủ dùng</t>
   </si>
   <si>
-    <t>Lá trà Oolong</t>
-  </si>
-  <si>
-    <t>Hạt Cà phê Robusta</t>
+    <t>Hạt Cà Phê Arabica (Nhập)</t>
+  </si>
+  <si>
+    <t>Siro Đào</t>
+  </si>
+  <si>
+    <t>chai</t>
+  </si>
+  <si>
+    <t>Hạt Cà Phê Robusta (VN)</t>
+  </si>
+  <si>
+    <t>Sữa tươi thanh trùng</t>
+  </si>
+  <si>
+    <t>lít</t>
   </si>
   <si>
     <t>Đường cát trắng</t>
   </si>
   <si>
-    <t>Sữa tươi không đường</t>
-  </si>
-  <si>
-    <t>lít</t>
+    <t>Sữa đặc Ông Thọ (lon)</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
+  <si>
+    <t>Trà túi lọc Lipton</t>
+  </si>
+  <si>
+    <t>túi</t>
   </si>
   <si>
     <t>Lịch sử Kiểm Kê (Chênh lệch)</t>
@@ -95,10 +113,13 @@
     <t>LyDoChenhLech</t>
   </si>
   <si>
-    <t>Hỏng</t>
-  </si>
-  <si>
-    <t>Rơi vãi</t>
+    <t>Thất lạc 2 túi</t>
+  </si>
+  <si>
+    <t>Hết hạn 1 lít</t>
+  </si>
+  <si>
+    <t>Hao hụt pha chế</t>
   </si>
   <si>
     <t>Lịch sử Hủy Hàng</t>
@@ -116,13 +137,28 @@
     <t>LyDoHuy</t>
   </si>
   <si>
-    <t>Rơi vỡ</t>
-  </si>
-  <si>
-    <t>Hết hạn sử dụng</t>
-  </si>
-  <si>
-    <t>Hư hỏng do vận chuyển</t>
+    <t>Hủy 2kg đường bị ướt</t>
+  </si>
+  <si>
+    <t>Hủy 1 lon sữa đặc móp</t>
+  </si>
+  <si>
+    <t>Hủy 0.1kg bột matcha ẩm mốc</t>
+  </si>
+  <si>
+    <t>Pha chế báo hỏng 1 chai siro đào</t>
+  </si>
+  <si>
+    <t>Hủy 0.05kg cafe hao hụt (sau kiểm kho 1)</t>
+  </si>
+  <si>
+    <t>Hủy 2 túi trà (sau kiểm kho 5)</t>
+  </si>
+  <si>
+    <t>Hủy nguyên liệu hỏng do trời mưa</t>
+  </si>
+  <si>
+    <t>Hủy 1 lít sữa tươi hết hạn (sau kiểm kho 2)</t>
   </si>
 </sst>
 </file>
@@ -290,8 +326,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:E8">
-  <autoFilter ref="A3:E8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:E11">
+  <autoFilter ref="A3:E11"/>
   <tableColumns count="5">
     <tableColumn id="1" name="TenNguyenLieu" totalsRowFunction="average"/>
     <tableColumn id="2" name="DonViTinh" totalsRowFunction="average"/>
@@ -304,8 +340,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:F5">
-  <autoFilter ref="A3:F5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:F6">
+  <autoFilter ref="A3:F6"/>
   <tableColumns count="6">
     <tableColumn id="1" name="NgayKiem" totalsRowFunction="average"/>
     <tableColumn id="2" name="TenNguyenLieu" totalsRowFunction="average"/>
@@ -319,8 +355,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:E6">
-  <autoFilter ref="A3:E6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:E11">
+  <autoFilter ref="A3:E11"/>
   <tableColumns count="5">
     <tableColumn id="1" name="NgayHuy" totalsRowFunction="average"/>
     <tableColumn id="2" name="TenNguyenLieu" totalsRowFunction="average"/>
@@ -341,7 +377,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.706134796142578" customWidth="1"/>
-    <col min="2" max="2" width="16.325510025024414" customWidth="1"/>
+    <col min="2" max="2" width="14.728787422180176" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -383,7 +419,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="9">
-        <v>15499999.9</v>
+        <v>4168600</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -401,7 +437,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="11">
-        <v>500000</v>
+        <v>407500</v>
       </c>
       <c r="C7" s="4"/>
     </row>
@@ -421,13 +457,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr ">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.30885887145996" customWidth="1"/>
+    <col min="1" max="1" width="26.31569480895996" customWidth="1"/>
     <col min="2" max="2" width="17.194204330444336" customWidth="1"/>
     <col min="3" max="3" width="17.194204330444336" customWidth="1"/>
     <col min="4" max="4" width="17.194204330444336" customWidth="1"/>
@@ -476,10 +512,10 @@
         <v>13</v>
       </c>
       <c r="C4" s="13">
-        <v>20</v>
+        <v>1.94</v>
       </c>
       <c r="D4" s="13">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>14</v>
@@ -493,10 +529,10 @@
         <v>13</v>
       </c>
       <c r="C5" s="13">
-        <v>30</v>
+        <v>4.76</v>
       </c>
       <c r="D5" s="13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>14</v>
@@ -507,13 +543,13 @@
         <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" s="13">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="D6" s="13">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>14</v>
@@ -521,16 +557,16 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="13">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="D7" s="13">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>14</v>
@@ -538,18 +574,69 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" s="13">
+        <v>10.2</v>
+      </c>
+      <c r="D8" s="13">
+        <v>5</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="13">
+        <v>19.86</v>
+      </c>
+      <c r="D9" s="13">
+        <v>5</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="13">
+        <v>48.79</v>
+      </c>
+      <c r="D10" s="13">
+        <v>10</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="13">
         <v>100</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D11" s="13">
         <v>20</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E11" s="0" t="s">
         <v>14</v>
       </c>
     </row>
@@ -557,7 +644,7 @@
   <mergeCells>
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A4:E8">
+  <conditionalFormatting sqref="A4:E11">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$E4="Hết hàng"</formula>
     </cfRule>
@@ -574,14 +661,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr ">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.194204330444336" customWidth="1"/>
-    <col min="2" max="2" width="22.30885887145996" customWidth="1"/>
+    <col min="2" max="2" width="24.753908157348633" customWidth="1"/>
     <col min="3" max="3" width="17.194204330444336" customWidth="1"/>
     <col min="4" max="4" width="17.194204330444336" customWidth="1"/>
     <col min="5" max="5" width="17.194204330444336" customWidth="1"/>
@@ -590,89 +677,109 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="14">
-        <v>45961.916666666664</v>
+        <v>45964</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C4" s="13">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="D4" s="13">
-        <v>29</v>
+        <v>98</v>
       </c>
       <c r="E4" s="13">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="14">
-        <v>45960.916666666664</v>
+        <v>45961</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="13">
+        <v>12</v>
+      </c>
+      <c r="D5" s="13">
+        <v>11</v>
+      </c>
+      <c r="E5" s="13">
+        <v>-1</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="14">
+        <v>45960</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="13">
-        <v>100</v>
-      </c>
-      <c r="D5" s="13">
-        <v>99.5</v>
-      </c>
-      <c r="E5" s="13">
-        <v>-0.5</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>27</v>
+      <c r="C6" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="E6" s="13">
+        <v>-0.05</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4:E5">
+  <conditionalFormatting sqref="E4:E6">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -689,109 +796,194 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr ">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.194204330444336" customWidth="1"/>
-    <col min="2" max="2" width="22.30885887145996" customWidth="1"/>
+    <col min="2" max="2" width="24.753908157348633" customWidth="1"/>
     <col min="3" max="3" width="17.194204330444336" customWidth="1"/>
     <col min="4" max="4" width="17.194204330444336" customWidth="1"/>
-    <col min="5" max="5" width="23.505708694458008" customWidth="1"/>
+    <col min="5" max="5" width="41.497947692871094" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="14">
-        <v>45952.666666666664</v>
+        <v>45968</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C4" s="13">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="3">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="14">
-        <v>45942.625</v>
+        <v>45967</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C5" s="13">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3">
-        <v>300000</v>
+        <v>30000</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="14">
-        <v>45933.583333333336</v>
+        <v>45966</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>40000</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="14">
+        <v>45965</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="13">
         <v>1</v>
       </c>
-      <c r="D6" s="3">
-        <v>133333</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>35</v>
+      <c r="D7" s="3">
+        <v>120000</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="14">
+        <v>45964</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="D8" s="3">
+        <v>12500</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="14">
+        <v>45963</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="13">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10000</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="14">
+        <v>45962</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>125000</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="14">
+        <v>45961</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="13">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>50000</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D4:D6">
+  <conditionalFormatting sqref="D4:D11">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>